<commit_message>
added boxplot for total frames
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/Train/Frames for P3.xlsx
+++ b/Dataset Excel Sheets/Frames/Train/Frames for P3.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaher.salman\Desktop\LINA JAN 24\Senior II\Senior-Design-Code\Dataset Excel Sheets\Frames\Train\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_05D1B5935BA0DC1337592911595ED87656CC120F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F63666D9-883B-40EB-89E3-8058E902FD67}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="100" windowWidth="21730" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,20 +473,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N539"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -501,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>45</v>
       </c>
@@ -534,7 +533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>51</v>
       </c>
@@ -569,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>54</v>
       </c>
@@ -604,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>49</v>
       </c>
@@ -639,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>53</v>
       </c>
@@ -671,7 +670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>58</v>
       </c>
@@ -700,7 +699,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>61</v>
       </c>
@@ -729,7 +728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>59</v>
       </c>
@@ -758,7 +757,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>66</v>
       </c>
@@ -787,7 +786,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>56</v>
       </c>
@@ -801,7 +800,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>58</v>
       </c>
@@ -815,7 +814,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>62</v>
       </c>
@@ -829,7 +828,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>59</v>
       </c>
@@ -843,7 +842,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>51</v>
       </c>
@@ -857,7 +856,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>47</v>
       </c>
@@ -871,7 +870,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>52</v>
       </c>
@@ -885,7 +884,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>48</v>
       </c>
@@ -899,7 +898,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>52</v>
       </c>
@@ -913,7 +912,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>53</v>
       </c>
@@ -927,7 +926,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>50</v>
       </c>
@@ -941,7 +940,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>51</v>
       </c>
@@ -955,7 +954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>47</v>
       </c>
@@ -969,7 +968,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>52</v>
       </c>
@@ -983,7 +982,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>51</v>
       </c>
@@ -997,7 +996,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>65</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>69</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>69</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>77</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>72</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>71</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>80</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>67</v>
       </c>
@@ -1109,7 +1108,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>59</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>68</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>68</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>67</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>61</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>56</v>
       </c>
@@ -1193,7 +1192,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>54</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>60</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>63</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>61</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>60</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>57</v>
       </c>
@@ -1277,7 +1276,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>59</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>59</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>56</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>52</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>62</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>59</v>
       </c>
@@ -1361,7 +1360,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>59</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>58</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>61</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>62</v>
       </c>
@@ -1417,7 +1416,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>63</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>69</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>67</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>69</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>70</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>77</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>72</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>64</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>72</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>57</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>66</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>67</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>62</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>62</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>70</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>64</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>65</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>57</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>69</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>91</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>85</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>82</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>92</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>86</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>83</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>81</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>90</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>86</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>84</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>80</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>87</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>70</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>71</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>62</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>66</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>66</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>69</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>64</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>66</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>62</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>68</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>73</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>71</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>68</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>76</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>92</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>87</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>90</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>80</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>93</v>
       </c>
@@ -2145,7 +2144,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>92</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>84</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>85</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>84</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>83</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>80</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>81</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>71</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>67</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>62</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>67</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>60</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>67</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>67</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>67</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>66</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>68</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>64</v>
       </c>
@@ -2397,7 +2396,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>65</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>60</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>70</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>69</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>71</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>69</v>
       </c>
@@ -2481,7 +2480,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>68</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>67</v>
       </c>
@@ -2509,7 +2508,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>71</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>74</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>68</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>71</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>85</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>76</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>72</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>75</v>
       </c>
@@ -2621,7 +2620,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>72</v>
       </c>
@@ -2635,7 +2634,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>71</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>74</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>77</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>55</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>52</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>57</v>
       </c>
@@ -2719,7 +2718,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>57</v>
       </c>
@@ -2733,7 +2732,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>55</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>59</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>57</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>54</v>
       </c>
@@ -2789,7 +2788,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>61</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>62</v>
       </c>
@@ -2817,7 +2816,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>60</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>57</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>63</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>59</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>54</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>54</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>63</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>53</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>63</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>52</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>47</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>50</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>59</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>55</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>51</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>51</v>
       </c>
@@ -3041,7 +3040,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>42</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>51</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>47</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>53</v>
       </c>
@@ -3097,7 +3096,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>52</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>54</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>48</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>48</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>50</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>46</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>46</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>85</v>
       </c>
@@ -3209,7 +3208,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>78</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>72</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>75</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>71</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>74</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>75</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>77</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>79</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>71</v>
       </c>
@@ -3335,7 +3334,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>73</v>
       </c>
@@ -3349,7 +3348,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>72</v>
       </c>
@@ -3363,7 +3362,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>81</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>85</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>86</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>93</v>
       </c>
@@ -3419,7 +3418,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>80</v>
       </c>
@@ -3433,7 +3432,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>79</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>86</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>90</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>95</v>
       </c>
@@ -3489,7 +3488,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>92</v>
       </c>
@@ -3503,7 +3502,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>89</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>92</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>85</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>101</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>80</v>
       </c>
@@ -3561,7 +3560,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>90</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>84</v>
       </c>
@@ -3583,7 +3582,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>83</v>
       </c>
@@ -3594,7 +3593,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>88</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>87</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>87</v>
       </c>
@@ -3627,7 +3626,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>89</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>83</v>
       </c>
@@ -3649,7 +3648,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>74</v>
       </c>
@@ -3660,7 +3659,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>75</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>81</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>73</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>64</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>61</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>70</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>72</v>
       </c>
@@ -3719,7 +3718,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>99</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>86</v>
       </c>
@@ -3735,7 +3734,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>71</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>71</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>68</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>72</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>77</v>
       </c>
@@ -3775,7 +3774,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>67</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>67</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>73</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>73</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>70</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>76</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>71</v>
       </c>
@@ -3831,7 +3830,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>96</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>88</v>
       </c>
@@ -3847,7 +3846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>84</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>87</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>86</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>94</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>87</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>85</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>82</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>79</v>
       </c>
@@ -3911,7 +3910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>80</v>
       </c>
@@ -3919,7 +3918,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>79</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>78</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>69</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>74</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>65</v>
       </c>
@@ -3959,7 +3958,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>66</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>60</v>
       </c>
@@ -3975,7 +3974,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>61</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>65</v>
       </c>
@@ -3991,7 +3990,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>63</v>
       </c>
@@ -3999,7 +3998,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>65</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>66</v>
       </c>
@@ -4015,7 +4014,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>66</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>62</v>
       </c>
@@ -4031,7 +4030,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>62</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>63</v>
       </c>
@@ -4047,7 +4046,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>61</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>62</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>69</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>90</v>
       </c>
@@ -4079,7 +4078,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>88</v>
       </c>
@@ -4087,7 +4086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>91</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>85</v>
       </c>
@@ -4103,7 +4102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>90</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>91</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>92</v>
       </c>
@@ -4127,7 +4126,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>84</v>
       </c>
@@ -4135,7 +4134,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>87</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>80</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>83</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>81</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>89</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>86</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>81</v>
       </c>
@@ -4191,7 +4190,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>87</v>
       </c>
@@ -4199,7 +4198,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>87</v>
       </c>
@@ -4207,7 +4206,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>84</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>79</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>73</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>80</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>83</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>75</v>
       </c>
@@ -4255,7 +4254,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>75</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>75</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>81</v>
       </c>
@@ -4279,7 +4278,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>79</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>77</v>
       </c>
@@ -4295,7 +4294,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>76</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>83</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>81</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>80</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>82</v>
       </c>
@@ -4335,7 +4334,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>78</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>84</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>81</v>
       </c>
@@ -4359,7 +4358,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>94</v>
       </c>
@@ -4367,7 +4366,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>79</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>81</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>80</v>
       </c>
@@ -4391,7 +4390,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>77</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>86</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>73</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>74</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>79</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>79</v>
       </c>
@@ -4439,7 +4438,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>73</v>
       </c>
@@ -4447,7 +4446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>75</v>
       </c>
@@ -4455,7 +4454,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>71</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>76</v>
       </c>
@@ -4471,7 +4470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>79</v>
       </c>
@@ -4479,7 +4478,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>110</v>
       </c>
@@ -4487,7 +4486,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>119</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>102</v>
       </c>
@@ -4503,7 +4502,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>102</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>86</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>93</v>
       </c>
@@ -4527,7 +4526,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>93</v>
       </c>
@@ -4535,7 +4534,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>107</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>105</v>
       </c>
@@ -4551,7 +4550,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>103</v>
       </c>
@@ -4559,7 +4558,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>90</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>96</v>
       </c>
@@ -4575,7 +4574,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>96</v>
       </c>
@@ -4583,7 +4582,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>94</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>82</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>83</v>
       </c>
@@ -4607,7 +4606,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>87</v>
       </c>
@@ -4615,7 +4614,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>88</v>
       </c>
@@ -4623,7 +4622,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>85</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>83</v>
       </c>
@@ -4639,7 +4638,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>75</v>
       </c>
@@ -4647,7 +4646,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>71</v>
       </c>
@@ -4655,7 +4654,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>67</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>70</v>
       </c>
@@ -4671,7 +4670,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>88</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>97</v>
       </c>
@@ -4687,7 +4686,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>97</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>98</v>
       </c>
@@ -4703,7 +4702,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>103</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>92</v>
       </c>
@@ -4719,7 +4718,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>95</v>
       </c>
@@ -4727,7 +4726,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>85</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>86</v>
       </c>
@@ -4743,7 +4742,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>92</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>91</v>
       </c>
@@ -4759,7 +4758,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>87</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>89</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>83</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>87</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>85</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>83</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>86</v>
       </c>
@@ -4815,7 +4814,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>87</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>85</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>87</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>93</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>94</v>
       </c>
@@ -4855,7 +4854,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>93</v>
       </c>
@@ -4863,7 +4862,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>112</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>111</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>113</v>
       </c>
@@ -4887,7 +4886,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>103</v>
       </c>
@@ -4895,7 +4894,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>104</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>92</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>101</v>
       </c>
@@ -4919,822 +4918,822 @@
         <v>126</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>104</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>99</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>95</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>95</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>103</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>101</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>91</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>92</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>99</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>89</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>96</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>94</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>86</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>95</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>81</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>89</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>100</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>81</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>75</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>69</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>91</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>88</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>84</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>69</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A400">
         <v>68</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A401">
         <v>80</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A402">
         <v>83</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A403">
         <v>79</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A404">
         <v>88</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A405">
         <v>78</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A406">
         <v>74</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A407">
         <v>73</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A408">
         <v>61</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A409">
         <v>93</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A410">
         <v>75</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A411">
         <v>78</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A412">
         <v>66</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A413">
         <v>64</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A414">
         <v>72</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A415">
         <v>80</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A416">
         <v>77</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A417">
         <v>98</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A418">
         <v>96</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A419">
         <v>109</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A420">
         <v>116</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A421">
         <v>104</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A422">
         <v>123</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A423">
         <v>103</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A424">
         <v>105</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A425">
         <v>103</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A426">
         <v>94</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A427">
         <v>108</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A428">
         <v>94</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A429">
         <v>87</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A430">
         <v>96</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A431">
         <v>92</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A432">
         <v>105</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A433">
         <v>93</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A434">
         <v>99</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A435">
         <v>99</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A436">
         <v>92</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A437">
         <v>83</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438">
         <v>102</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A439">
         <v>79</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A440">
         <v>71</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A441">
         <v>88</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A442">
         <v>94</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A443">
         <v>82</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A444">
         <v>89</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A445">
         <v>89</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A446">
         <v>83</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A447">
         <v>85</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A448">
         <v>87</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A449">
         <v>74</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A450">
         <v>86</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A451">
         <v>82</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A452">
         <v>85</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A453">
         <v>89</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A454">
         <v>82</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A455">
         <v>82</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A456">
         <v>81</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A457">
         <v>83</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A458">
         <v>86</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A459">
         <v>82</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A460">
         <v>76</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A461">
         <v>92</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A462">
         <v>85</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A463">
         <v>83</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A464">
         <v>89</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A465">
         <v>83</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A466">
         <v>82</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A467">
         <v>74</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A468">
         <v>72</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A469">
         <v>79</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A470">
         <v>74</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A471">
         <v>70</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A472">
         <v>74</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A473">
         <v>71</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A474">
         <v>81</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A475">
         <v>57</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A476">
         <v>62</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A477">
         <v>81</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A478">
         <v>85</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A479">
         <v>72</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A480">
         <v>75</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A481">
         <v>71</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A482">
         <v>75</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A483">
         <v>74</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A484">
         <v>67</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A485">
         <v>87</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A486">
         <v>82</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A487">
         <v>82</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A488">
         <v>64</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A489">
         <v>78</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A490">
         <v>82</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A491">
         <v>77</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A492">
         <v>71</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A493">
         <v>74</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A494">
         <v>73</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A495">
         <v>74</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A496">
         <v>63</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A497">
         <v>85</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A498">
         <v>74</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A499">
         <v>74</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A500">
         <v>88</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A501">
         <v>74</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A502">
         <v>71</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A503">
         <v>58</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A504">
         <v>73</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A505">
         <v>58</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A506">
         <v>70</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A507">
         <v>75</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A508">
         <v>75</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A509">
         <v>67</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A510">
         <v>79</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A511">
         <v>72</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A512">
         <v>65</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A513">
         <v>70</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A514">
         <v>58</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A515">
         <v>77</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A516">
         <v>71</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A517">
         <v>63</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A518">
         <v>65</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A519">
         <v>71</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A520">
         <v>75</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A521">
         <v>67</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A522">
         <v>70</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A523">
         <v>65</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A524">
         <v>67</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A525">
         <v>74</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A526">
         <v>70</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A527">
         <v>72</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A528">
         <v>70</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A529">
         <v>69</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A530">
         <v>56</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A531">
         <v>69</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A532">
         <v>59</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A533">
         <v>59</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A534">
         <v>51</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A535">
         <v>60</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A536">
         <v>47</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A537">
         <v>51</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A538">
         <v>64</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A539">
         <v>77</v>
       </c>

</xml_diff>